<commit_message>
Updated the issue list
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="11475" windowHeight="4620"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="11472" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -238,12 +238,30 @@
   <si>
     <t>Test Classes missing for StoreKeeper, Discount and Member/Customer</t>
   </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Add first transaction without selecting the product (click '+' button)</t>
+  </si>
+  <si>
+    <t>Click '+' button showing the confirm dialog box "Do you want to delete the item from the list?" and clicks cancel throws exception</t>
+  </si>
+  <si>
+    <t>Sabethan</t>
+  </si>
+  <si>
+    <t>Fixed Remark</t>
+  </si>
+  <si>
+    <t>Test class added for storekeeper</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -329,6 +347,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +439,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -453,7 +473,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -629,24 +648,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="52.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="39.88671875" style="5" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="13.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="28.8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -671,8 +692,11 @@
       <c r="H1" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -689,7 +713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="84.75" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -709,7 +733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -726,7 +750,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -746,7 +770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="43.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -766,7 +790,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="43.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -786,7 +810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -803,7 +827,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="43.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -821,7 +845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -838,7 +862,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -856,7 +880,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -873,7 +897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="57.6">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -891,7 +915,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.8">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -908,7 +932,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="3" customFormat="1">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -926,7 +950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -943,7 +967,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -961,7 +985,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -978,7 +1002,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -996,7 +1020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.8">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1010,7 +1034,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1028,7 +1052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1045,7 +1069,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1061,7 +1085,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1075,7 +1099,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="28.8">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1091,7 +1115,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1105,7 +1129,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="43.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1117,6 +1141,29 @@
       </c>
       <c r="F27" s="6" t="s">
         <v>59</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="43.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1126,24 +1173,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Issues .xls with status. Several issues have been fixed (Refer xls for details). Three issues are work in progress and I have marked them as WIP in status.
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\NUS\src\SouvenirStore\internal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="180" windowWidth="11475" windowHeight="4620"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="108">
   <si>
     <t>#</t>
   </si>
@@ -346,6 +351,44 @@
   </si>
   <si>
     <t>This MemberDiscount is extended to compute the appropriate discount value</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Nikhil</t>
+  </si>
+  <si>
+    <t>Fixed the exception by adding null check before trying to loop through vendors.
+I tried to display the arrow but it requires a custom draw method. Given the time constraint, I think it's not a priority.</t>
+  </si>
+  <si>
+    <t>Not Fixed</t>
+  </si>
+  <si>
+    <t>I removed this when I implemented Jtable UI. Although I have it on my mind to add it back, I think this is low priority since this functionality does not serve any real purpose.</t>
+  </si>
+  <si>
+    <t>Disabled multi select</t>
+  </si>
+  <si>
+    <t>In AddProduct dialog, the Product Id displayer will be &lt;CATEGORY CODE&gt;/ without any sequence number.
+After clicking add button, a new sequence number is generated. Thus avoiding creation of throwaway sequence numbers.</t>
+  </si>
+  <si>
+    <t>If the product is not available, the quantity can be made 0</t>
+  </si>
+  <si>
+    <t>Renamed column titles and removed category column</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>I conside this low priority. Currently all dialogs are set to display on center of screen.</t>
+  </si>
+  <si>
+    <t>This is fixed in issue 5 above.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +547,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,7 +582,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -750,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,6 +855,12 @@
       <c r="F2" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -832,9 +881,17 @@
       <c r="F3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -849,6 +906,15 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -870,9 +936,17 @@
       <c r="F5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -890,6 +964,15 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -911,9 +994,15 @@
       <c r="F7" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -928,6 +1017,15 @@
       </c>
       <c r="F8" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -947,7 +1045,15 @@
       <c r="F9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="G9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1287,7 +1393,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1299,6 +1405,12 @@
       </c>
       <c r="F29" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="I29" s="8">
         <v>3</v>
@@ -1320,6 +1432,12 @@
       <c r="F30" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="I30" s="8">
         <v>5</v>
       </c>
@@ -1337,8 +1455,11 @@
       <c r="F31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I31" s="8">
-        <v>5</v>
+      <c r="H31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1357,8 +1478,14 @@
       <c r="F32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I32" s="8">
-        <v>4</v>
+      <c r="G32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -1384,6 +1511,12 @@
       </c>
       <c r="F34" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="I34" s="8">
         <v>3</v>

</xml_diff>

<commit_message>
Added code length check in AddCategoryDialog. If code length is less or more than three characters, an exception is thrown. Added logic to handle the exception.
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="109">
   <si>
     <t>#</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>This is fixed in issue 5 above.</t>
+  </si>
+  <si>
+    <t>Added code length check in AddCategory dialog. If code length is less or more than three characters, an exception is thrown. Added logic to handle the exception.</t>
   </si>
 </sst>
 </file>
@@ -794,7 +797,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1396,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1407,13 +1410,13 @@
         <v>69</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I29" s="8">
-        <v>3</v>
+      <c r="I29" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reported two window resize issues related to Transaction UI
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\NUS\src\SouvenirStore\internal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NUS\Source\SouvenirStore\internal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="114">
   <si>
     <t>#</t>
   </si>
@@ -392,6 +392,31 @@
   </si>
   <si>
     <t>Added code length check in AddCategory dialog. If code length is less or more than three characters, an exception is thrown. Added logic to handle the exception.</t>
+  </si>
+  <si>
+    <t>Transaction UI</t>
+  </si>
+  <si>
+    <t>Resizing main window does not resize Transaction panels accordingly.</t>
+  </si>
+  <si>
+    <t>Clicking View button, resets size of main window.</t>
+  </si>
+  <si>
+    <t>Case 1:
+Select Reports-&gt;Transactions
+Maximize main app window
+Observe that Transaction panel does not resizeaccordingly
+Case 2:
+Instead of maximizing the window, reduce the size.
+Observe that the UI is clipped.</t>
+  </si>
+  <si>
+    <t>Maximize main app window
+Select Reports-&gt;Transactions
+Click search
+Select transaction from list and click View button
+Observe that the main window size is reset</t>
   </si>
 </sst>
 </file>
@@ -794,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1516,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1505,7 +1533,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
@@ -1525,7 +1556,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1539,7 +1573,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>43</v>
       </c>
@@ -1553,7 +1590,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
       <c r="B37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1570,7 +1610,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
       <c r="B38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1581,7 +1624,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
       <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
@@ -1607,7 +1653,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
       <c r="B40" s="1" t="s">
         <v>83</v>
       </c>
@@ -1627,7 +1676,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
       <c r="B41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1645,6 +1697,90 @@
       </c>
       <c r="I41" s="8" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resetting transaction details window according to the main window.
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="3984"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11688" windowHeight="3984"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="122">
   <si>
     <t>#</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>Issue fixed as per point 24</t>
+  </si>
+  <si>
+    <t>Resetting size of the transaction detail window done according to the main window.</t>
   </si>
 </sst>
 </file>
@@ -838,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,7 +1802,13 @@
         <v>97</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed issue: Vendor name must be unique.
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NUS\Source\SouvenirStore\internal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11688" windowHeight="3984"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11685" windowHeight="3990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="123">
   <si>
     <t>#</t>
   </si>
@@ -437,12 +442,15 @@
   <si>
     <t>Resetting size of the transaction detail window done according to the main window.</t>
   </si>
+  <si>
+    <t>Updated logic to check whether the vendor already exists.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,7 +602,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,9 +634,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -660,6 +669,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -835,27 +845,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="5" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="38" style="5" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="8.85546875" style="1"/>
     <col min="9" max="9" width="46" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="28.8">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +894,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -907,7 +917,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="84.75" customHeight="1">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -936,7 +946,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -962,7 +972,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="28.8">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -991,7 +1001,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="72">
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="57.6">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1047,7 +1057,7 @@
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="28.8">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="43.2">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1100,7 +1110,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1">
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1136,7 +1146,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" ht="28.8">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1153,7 +1163,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="57.6">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1172,7 +1182,7 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" ht="28.8">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1189,7 +1199,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1208,7 +1218,7 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="28.8">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1244,7 +1254,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="28.8">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1286,7 +1296,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" ht="28.8">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1300,7 +1310,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" ht="43.2">
+    <row r="21" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1319,7 +1329,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" ht="28.8">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1345,7 +1355,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="43.2">
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1367,7 +1377,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1390,7 +1400,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" ht="28.8">
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1415,7 +1425,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="28.8">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1438,7 +1448,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" ht="28.8">
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="43.2">
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1484,7 +1494,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="57.6">
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="57.6">
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1524,16 +1534,16 @@
         <v>69</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I30" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="28.8">
+      <c r="I30" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="43.2">
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1596,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="28.8">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1619,7 +1629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1636,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1659,7 +1669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1685,7 +1695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="28.8">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1734,7 +1744,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="57.6">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1757,7 +1767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="94.5" customHeight="1">
+    <row r="41" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1780,7 +1790,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="129.6">
+    <row r="42" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1806,7 +1816,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="72">
+    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1832,52 +1842,52 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1889,24 +1899,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed issue: - Duplicate category addition. New behavior: Error message pops up if category already exists.
</commit_message>
<xml_diff>
--- a/SouvenirStore/internal/Issues.xlsx
+++ b/SouvenirStore/internal/Issues.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="123">
   <si>
     <t>#</t>
   </si>
@@ -382,9 +382,6 @@
     <t>Renamed column titles and removed category column</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t>I conside this low priority. Currently all dialogs are set to display on center of screen.</t>
   </si>
   <si>
@@ -444,6 +441,9 @@
   </si>
   <si>
     <t>Updated logic to check whether the vendor already exists.</t>
+  </si>
+  <si>
+    <t>Added duplicate check for category</t>
   </si>
 </sst>
 </file>
@@ -849,7 +849,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,10 +1349,10 @@
         <v>96</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>99</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1394,10 +1394,10 @@
         <v>96</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>96</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1442,10 +1442,10 @@
         <v>96</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>97</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
         <v>97</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>97</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>97</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1620,13 +1620,13 @@
         <v>69</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="8">
-        <v>3</v>
+      <c r="I34" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1795,13 +1795,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>97</v>
@@ -1810,10 +1810,10 @@
         <v>96</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1821,13 +1821,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>97</v>
@@ -1836,10 +1836,10 @@
         <v>96</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>